<commit_message>
Try to make export
</commit_message>
<xml_diff>
--- a/my_data.xlsx
+++ b/my_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hosgl\PycharmProjects\courseProgMethods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\courseProgMethods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABB026D-C72C-4845-9598-CBA3D1E88887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A2409D-84CC-4EE9-91E4-8B5FB7AD1EEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Edges" sheetId="1" r:id="rId1"/>
@@ -1290,17 +1290,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" zoomScale="115" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F243" sqref="F243"/>
+    <sheetView zoomScale="115" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>82</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>87</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>89</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>91</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>93</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>94</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>95</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>98</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>99</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>100</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>101</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>90</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>92</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>103</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>105</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>107</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>109</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>111</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>112</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>113</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>114</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>115</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>116</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>117</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>118</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>119</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>121</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>123</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>124</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>125</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>126</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>128</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>130</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>131</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>132</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>133</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>134</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>135</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>136</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>137</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>139</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>141</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>68</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>143</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>144</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>145</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>145</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>146</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>147</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>148</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>22</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>24</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>96</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>102</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>150</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>151</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>151</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>26</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>120</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>104</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>106</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>108</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>110</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>154</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>129</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>153</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>155</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>156</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>157</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>158</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>159</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>160</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>161</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>162</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>163</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>164</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>165</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>127</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>152</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>152</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>167</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>168</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>169</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>170</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>171</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>138</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>172</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>173</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>174</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>175</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>176</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>177</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>178</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>179</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>180</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>181</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>182</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>183</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>184</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>185</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>186</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>187</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>188</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>189</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>190</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>191</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>192</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>193</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>194</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>195</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>196</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>197</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>198</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>199</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>200</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>201</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>202</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>203</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>204</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>205</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>206</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>207</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>208</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>210</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>211</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>212</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>213</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>214</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>216</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>218</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>219</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>220</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>221</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>222</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>223</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>224</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>226</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>227</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>228</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>229</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>230</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>231</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>232</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>233</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>235</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>235</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>237</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>237</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>238</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>238</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>238</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>239</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>240</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>241</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>242</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>86</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>243</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>244</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>245</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>246</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>247</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>248</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>249</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>249</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>250</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>251</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>252</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>253</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>254</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>255</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>256</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>257</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>88</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>258</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>259</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>261</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>262</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>263</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>264</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>266</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>266</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>268</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>269</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>270</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>272</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>274</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>275</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>276</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>277</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>260</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>279</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>280</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>281</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>282</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>283</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>44</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>284</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>28</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>28</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>28</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>28</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>28</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>28</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>28</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>28</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>28</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>28</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>28</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>28</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>28</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>28</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>28</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>28</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>286</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>13</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>13</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>288</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>63</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>64</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>209</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>225</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>234</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>28</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>66</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>67</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>68</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>68</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>71</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>71</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>74</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>290</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>76</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A249" s="3" t="s">
         <v>82</v>
       </c>
@@ -3303,17 +3303,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E21D01C-9876-4D06-B4E3-910DFDDF6C77}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>83</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>285</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>50</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>51</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>287</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>60</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>61</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>54</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>32</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>35</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>291</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>140</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>72</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>73</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>69</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>77</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>14</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>70</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>38</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>21</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>11</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>37</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>286</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>29</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>62</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>15</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>16</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>17</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>18</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>55</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>47</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>42</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>65</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>27</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>56</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>49</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>57</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>58</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>59</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>36</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>25</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>76</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>31</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>82</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>236</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>292</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>28</v>
       </c>

</xml_diff>